<commit_message>
changed to orders, cartons and mikeExperiment
</commit_message>
<xml_diff>
--- a/asn_greaterThan100Cases.xlsx
+++ b/asn_greaterThan100Cases.xlsx
@@ -644,7 +644,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4.2</v>
+        <v>4.199999999999999</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>100</v>
@@ -708,7 +708,7 @@
         <v>214</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>187.28000000000003</v>
+        <v>187.28</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>4494</v>
@@ -740,7 +740,7 @@
         <v>235</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>144.74999999999997</v>
+        <v>144.7499999999999</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3471</v>
@@ -772,7 +772,7 @@
         <v>185</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>117.22000000000001</v>
+        <v>117.22000000000003</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>2811</v>
@@ -836,7 +836,7 @@
         <v>118</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>50.620000000000005</v>
+        <v>50.62000000000002</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1213</v>
@@ -868,7 +868,7 @@
         <v>461</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>291.65</v>
+        <v>291.6499999999999</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>6996</v>
@@ -900,7 +900,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>14.360000000000003</v>
+        <v>14.360000000000001</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>344</v>
@@ -932,7 +932,7 @@
         <v>180</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>125.6</v>
+        <v>125.59999999999998</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>3014</v>
@@ -996,7 +996,7 @@
         <v>175</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>92.52000000000005</v>
+        <v>92.5200000000001</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>2219</v>
@@ -1028,7 +1028,7 @@
         <v>269</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>220.81</v>
+        <v>220.81000000000006</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>5299</v>
@@ -1060,7 +1060,7 @@
         <v>276</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>145.04999999999995</v>
+        <v>145.04999999999987</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>3479</v>
@@ -1092,7 +1092,7 @@
         <v>115</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>42.94000000000001</v>
+        <v>42.94</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1029</v>
@@ -1124,7 +1124,7 @@
         <v>357</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>211.33999999999978</v>
+        <v>211.3399999999998</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>5070</v>
@@ -1188,7 +1188,7 @@
         <v>232</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>148.73999999999995</v>
+        <v>148.73999999999998</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>3567</v>
@@ -1220,7 +1220,7 @@
         <v>120</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>90.57000000000001</v>
+        <v>90.57</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>2173</v>
@@ -1252,7 +1252,7 @@
         <v>301</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>193.36999999999998</v>
+        <v>193.36999999999995</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>4638</v>
@@ -1284,7 +1284,7 @@
         <v>452</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>369.01</v>
+        <v>369.00999999999993</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>8853</v>
@@ -1316,7 +1316,7 @@
         <v>445</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>322.3899999999998</v>
+        <v>322.3899999999999</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>7734</v>
@@ -1348,7 +1348,7 @@
         <v>402</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>179.65000000000006</v>
+        <v>179.6500000000001</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>4309</v>
@@ -1380,7 +1380,7 @@
         <v>643</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>511.33</v>
+        <v>511.33000000000004</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>12269</v>
@@ -1412,7 +1412,7 @@
         <v>311</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>156.67999999999986</v>
+        <v>156.67999999999984</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>3755</v>
@@ -1444,7 +1444,7 @@
         <v>111</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>98.22000000000001</v>
+        <v>98.22000000000003</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>2357</v>
@@ -1476,7 +1476,7 @@
         <v>202</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>150.29</v>
+        <v>150.28999999999996</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>3606</v>
@@ -1540,7 +1540,7 @@
         <v>339</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>216.70999999999998</v>
+        <v>216.70999999999995</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>5198</v>
@@ -1572,7 +1572,7 @@
         <v>331</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>267.6</v>
+        <v>267.59999999999997</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>6421</v>
@@ -1636,7 +1636,7 @@
         <v>239</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>222.54</v>
+        <v>222.54000000000002</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>5340</v>
@@ -1668,7 +1668,7 @@
         <v>271</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>174.8699999999999</v>
+        <v>174.86999999999998</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>4194</v>
@@ -1700,7 +1700,7 @@
         <v>480</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>277.9300000000002</v>
+        <v>277.92999999999955</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>6665</v>
@@ -1732,7 +1732,7 @@
         <v>108</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>55.89000000000001</v>
+        <v>55.890000000000015</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>1340</v>
@@ -1796,7 +1796,7 @@
         <v>304</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>170.82999999999996</v>
+        <v>170.82999999999993</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>4098</v>
@@ -1828,7 +1828,7 @@
         <v>260</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>73.71000000000004</v>
+        <v>73.71</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>1766</v>
@@ -1860,7 +1860,7 @@
         <v>465</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>345.5499999999998</v>
+        <v>345.54999999999984</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>8290</v>
@@ -1924,7 +1924,7 @@
         <v>155</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>70.7</v>
+        <v>70.69999999999999</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>1694</v>
@@ -1956,7 +1956,7 @@
         <v>430</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>251.56999999999974</v>
+        <v>251.56999999999977</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>6033</v>
@@ -2052,7 +2052,7 @@
         <v>186</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>103.01999999999997</v>
+        <v>103.02</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>2471</v>
@@ -2148,7 +2148,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>35.92</v>
+        <v>35.919999999999995</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>861</v>
@@ -2180,7 +2180,7 @@
         <v>267</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>198.02999999999992</v>
+        <v>198.02999999999997</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>4750</v>
@@ -2212,7 +2212,7 @@
         <v>209</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>128.69000000000005</v>
+        <v>128.69000000000008</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>3087</v>
@@ -2308,7 +2308,7 @@
         <v>48</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>30.450000000000003</v>
+        <v>30.45</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>730</v>
@@ -2404,7 +2404,7 @@
         <v>192</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>147.86000000000004</v>
+        <v>147.85999999999999</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>3548</v>
@@ -2468,7 +2468,7 @@
         <v>268</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>161.07999999999996</v>
+        <v>161.07999999999998</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>3864</v>
@@ -2596,7 +2596,7 @@
         <v>287</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>209.40000000000003</v>
+        <v>209.4</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>5025</v>
@@ -2628,7 +2628,7 @@
         <v>184</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>124.62999999999995</v>
+        <v>124.62999999999998</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>2989</v>
@@ -2660,7 +2660,7 @@
         <v>66</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>23.729999999999993</v>
+        <v>23.729999999999997</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>569</v>
@@ -2692,7 +2692,7 @@
         <v>503</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>272.0599999999998</v>
+        <v>272.0599999999999</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>6525</v>
@@ -2724,7 +2724,7 @@
         <v>93</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>52.980000000000004</v>
+        <v>52.98</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>1271</v>
@@ -2788,7 +2788,7 @@
         <v>188</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>146.27</v>
+        <v>146.27000000000004</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>3510</v>
@@ -2820,7 +2820,7 @@
         <v>104</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>76.00999999999999</v>
+        <v>76.00999999999998</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>1824</v>
@@ -2884,7 +2884,7 @@
         <v>259</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>122.48999999999997</v>
+        <v>122.48999999999995</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>2937</v>
@@ -2916,7 +2916,7 @@
         <v>246</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>123.24000000000015</v>
+        <v>123.24000000000014</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>2955</v>
@@ -2948,7 +2948,7 @@
         <v>287</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>166.63999999999993</v>
+        <v>166.63999999999996</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>3998</v>
@@ -2980,7 +2980,7 @@
         <v>282</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>155.7999999999998</v>
+        <v>155.79999999999993</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>3738</v>
@@ -3044,7 +3044,7 @@
         <v>45</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>34.529999999999994</v>
+        <v>34.53</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>829</v>
@@ -3076,7 +3076,7 @@
         <v>524</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>269.2399999999997</v>
+        <v>269.23999999999967</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>6459</v>
@@ -3204,7 +3204,7 @@
         <v>353</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>202.7899999999997</v>
+        <v>202.78999999999985</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>4863</v>
@@ -3268,7 +3268,7 @@
         <v>220</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>142.79</v>
+        <v>142.79000000000002</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>3425</v>
@@ -3332,7 +3332,7 @@
         <v>169</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>63.7</v>
+        <v>63.70000000000001</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>1527</v>
@@ -3396,7 +3396,7 @@
         <v>211</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>143.29</v>
+        <v>143.28999999999994</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>3438</v>
@@ -3524,7 +3524,7 @@
         <v>177</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>84.29</v>
+        <v>84.28999999999996</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>2021</v>
@@ -3556,7 +3556,7 @@
         <v>67</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>31.149999999999995</v>
+        <v>31.150000000000002</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>746</v>
@@ -3588,7 +3588,7 @@
         <v>121</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>67.92000000000002</v>
+        <v>67.92000000000003</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>1628</v>
@@ -3620,7 +3620,7 @@
         <v>210</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>123.21999999999993</v>
+        <v>123.21999999999991</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>2957</v>
@@ -3716,7 +3716,7 @@
         <v>27</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>13.450000000000001</v>
+        <v>13.45</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>322</v>
@@ -3748,7 +3748,7 @@
         <v>179</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>42.09</v>
+        <v>42.090000000000025</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>1006</v>
@@ -3812,7 +3812,7 @@
         <v>86</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>42.320000000000014</v>
+        <v>42.31999999999999</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>1014</v>
@@ -3876,7 +3876,7 @@
         <v>290</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>193.92999999999995</v>
+        <v>193.92999999999992</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>4654</v>
@@ -3908,7 +3908,7 @@
         <v>81</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>33.54999999999999</v>
+        <v>33.55</v>
       </c>
       <c r="E108" s="0" t="n">
         <v>804</v>
@@ -3972,7 +3972,7 @@
         <v>463</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>301.3499999999999</v>
+        <v>301.3499999999998</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>7227</v>
@@ -4004,7 +4004,7 @@
         <v>239</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>195.9999999999999</v>
+        <v>195.99999999999994</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>4703</v>
@@ -4068,7 +4068,7 @@
         <v>57</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>39.08999999999999</v>
+        <v>39.089999999999996</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>938</v>
@@ -4100,7 +4100,7 @@
         <v>240</v>
       </c>
       <c r="D114" s="0" t="n">
-        <v>165.25000000000006</v>
+        <v>165.25000000000003</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>3965</v>
@@ -4132,7 +4132,7 @@
         <v>242</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>133.95000000000007</v>
+        <v>133.95000000000002</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>3214</v>
@@ -4164,7 +4164,7 @@
         <v>212</v>
       </c>
       <c r="D116" s="0" t="n">
-        <v>87.61000000000004</v>
+        <v>87.61000000000001</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>2100</v>
@@ -4196,7 +4196,7 @@
         <v>270</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>166.00000000000003</v>
+        <v>166.00000000000009</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>3982</v>
@@ -4228,7 +4228,7 @@
         <v>130</v>
       </c>
       <c r="D118" s="0" t="n">
-        <v>116.3</v>
+        <v>116.30000000000003</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>2791</v>
@@ -4260,7 +4260,7 @@
         <v>53</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>43.309999999999995</v>
+        <v>43.31</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>1039</v>
@@ -4292,7 +4292,7 @@
         <v>59</v>
       </c>
       <c r="D120" s="0" t="n">
-        <v>37.39</v>
+        <v>37.39000000000001</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>896</v>
@@ -4516,7 +4516,7 @@
         <v>112</v>
       </c>
       <c r="D127" s="0" t="n">
-        <v>40.83</v>
+        <v>40.830000000000005</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>978</v>
@@ -4580,7 +4580,7 @@
         <v>32</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>6.170000000000001</v>
+        <v>6.17</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>148</v>
@@ -4612,7 +4612,7 @@
         <v>37</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>25.869999999999997</v>
+        <v>25.869999999999994</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>621</v>

</xml_diff>

<commit_message>
changes to dailyReceving, orders, vas
</commit_message>
<xml_diff>
--- a/asn_greaterThan100Cases.xlsx
+++ b/asn_greaterThan100Cases.xlsx
@@ -6,12 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="greaterThan100Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="volBands" sheetId="2" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>Date</t>
   </si>
@@ -428,6 +429,30 @@
   </si>
   <si>
     <t>20200327</t>
+  </si>
+  <si>
+    <t>volBand</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>skus</t>
+  </si>
+  <si>
+    <t>shipments</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -505,7 +530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:8">
       <c r="A2" s="0" t="s">
         <v>10</v>
       </c>
@@ -530,14 +555,8 @@
       <c r="H2" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>139</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
@@ -562,14 +581,8 @@
       <c r="H3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>135</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -594,14 +607,8 @@
       <c r="H4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>287</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -626,14 +633,8 @@
       <c r="H5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J5" s="0" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="0" t="s">
         <v>14</v>
       </c>
@@ -644,7 +645,7 @@
         <v>17</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>4.199999999999999</v>
+        <v>4.2</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>100</v>
@@ -658,14 +659,8 @@
       <c r="H6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="0" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
@@ -690,14 +685,8 @@
       <c r="H7" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <v>191</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="0" t="s">
         <v>16</v>
       </c>
@@ -708,7 +697,7 @@
         <v>214</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>187.28</v>
+        <v>187.28000000000003</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>4494</v>
@@ -722,14 +711,8 @@
       <c r="H8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>195</v>
-      </c>
-      <c r="J8" s="0" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="0" t="s">
         <v>17</v>
       </c>
@@ -740,7 +723,7 @@
         <v>235</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>144.7499999999999</v>
+        <v>144.74999999999997</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3471</v>
@@ -754,14 +737,8 @@
       <c r="H9" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I9" s="0" t="n">
-        <v>158</v>
-      </c>
-      <c r="J9" s="0" t="n">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
@@ -772,7 +749,7 @@
         <v>185</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>117.22000000000003</v>
+        <v>117.22000000000001</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>2811</v>
@@ -786,14 +763,8 @@
       <c r="H10" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="I10" s="0" t="n">
-        <v>124</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="0" t="s">
         <v>19</v>
       </c>
@@ -818,14 +789,8 @@
       <c r="H11" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="I11" s="0" t="n">
-        <v>405</v>
-      </c>
-      <c r="J11" s="0" t="n">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="0" t="s">
         <v>20</v>
       </c>
@@ -836,7 +801,7 @@
         <v>118</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>50.62000000000002</v>
+        <v>50.620000000000005</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1213</v>
@@ -850,14 +815,8 @@
       <c r="H12" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I12" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="J12" s="0" t="n">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="0" t="s">
         <v>21</v>
       </c>
@@ -868,7 +827,7 @@
         <v>461</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>291.6499999999999</v>
+        <v>291.65</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>6996</v>
@@ -882,14 +841,8 @@
       <c r="H13" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>317</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="0" t="s">
         <v>22</v>
       </c>
@@ -900,7 +853,7 @@
         <v>35</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>14.360000000000001</v>
+        <v>14.360000000000003</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>344</v>
@@ -914,14 +867,8 @@
       <c r="H14" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="0" t="s">
         <v>23</v>
       </c>
@@ -932,7 +879,7 @@
         <v>180</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>125.59999999999998</v>
+        <v>125.6</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>3014</v>
@@ -946,14 +893,8 @@
       <c r="H15" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I15" s="0" t="n">
-        <v>137</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="0" t="s">
         <v>24</v>
       </c>
@@ -978,14 +919,8 @@
       <c r="H16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I16" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="0" t="s">
         <v>25</v>
       </c>
@@ -996,7 +931,7 @@
         <v>175</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>92.5200000000001</v>
+        <v>92.52000000000005</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>2219</v>
@@ -1010,14 +945,8 @@
       <c r="H17" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="I17" s="0" t="n">
-        <v>101</v>
-      </c>
-      <c r="J17" s="0" t="n">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="0" t="s">
         <v>26</v>
       </c>
@@ -1028,7 +957,7 @@
         <v>269</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>220.81000000000006</v>
+        <v>220.81</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>5299</v>
@@ -1042,14 +971,8 @@
       <c r="H18" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I18" s="0" t="n">
-        <v>250</v>
-      </c>
-      <c r="J18" s="0" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="0" t="s">
         <v>27</v>
       </c>
@@ -1060,7 +983,7 @@
         <v>276</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>145.04999999999987</v>
+        <v>145.04999999999995</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>3479</v>
@@ -1074,14 +997,8 @@
       <c r="H19" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I19" s="0" t="n">
-        <v>156</v>
-      </c>
-      <c r="J19" s="0" t="n">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="0" t="s">
         <v>28</v>
       </c>
@@ -1092,7 +1009,7 @@
         <v>115</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>42.94</v>
+        <v>42.94000000000001</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1029</v>
@@ -1106,14 +1023,8 @@
       <c r="H20" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I20" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="J20" s="0" t="n">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="0" t="s">
         <v>29</v>
       </c>
@@ -1124,7 +1035,7 @@
         <v>357</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>211.3399999999998</v>
+        <v>211.33999999999978</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>5070</v>
@@ -1138,14 +1049,8 @@
       <c r="H21" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="I21" s="0" t="n">
-        <v>228</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="0" t="s">
         <v>30</v>
       </c>
@@ -1170,14 +1075,8 @@
       <c r="H22" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I22" s="0" t="n">
-        <v>177</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="0" t="s">
         <v>31</v>
       </c>
@@ -1188,7 +1087,7 @@
         <v>232</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>148.73999999999998</v>
+        <v>148.73999999999995</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>3567</v>
@@ -1202,14 +1101,8 @@
       <c r="H23" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="I23" s="0" t="n">
-        <v>166</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="0" t="s">
         <v>32</v>
       </c>
@@ -1220,7 +1113,7 @@
         <v>120</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>90.57</v>
+        <v>90.57000000000001</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>2173</v>
@@ -1234,14 +1127,8 @@
       <c r="H24" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I24" s="0" t="n">
-        <v>109</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="0" t="s">
         <v>33</v>
       </c>
@@ -1252,7 +1139,7 @@
         <v>301</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>193.36999999999995</v>
+        <v>193.36999999999998</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>4638</v>
@@ -1266,14 +1153,8 @@
       <c r="H25" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I25" s="0" t="n">
-        <v>213</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="0" t="s">
         <v>34</v>
       </c>
@@ -1284,7 +1165,7 @@
         <v>452</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>369.00999999999993</v>
+        <v>369.01</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>8853</v>
@@ -1298,14 +1179,8 @@
       <c r="H26" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I26" s="0" t="n">
-        <v>393</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="0" t="s">
         <v>35</v>
       </c>
@@ -1316,7 +1191,7 @@
         <v>445</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>322.3899999999999</v>
+        <v>322.3899999999998</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>7734</v>
@@ -1330,14 +1205,8 @@
       <c r="H27" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I27" s="0" t="n">
-        <v>354</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="0" t="s">
         <v>36</v>
       </c>
@@ -1348,7 +1217,7 @@
         <v>402</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>179.6500000000001</v>
+        <v>179.65000000000006</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>4309</v>
@@ -1362,14 +1231,8 @@
       <c r="H28" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="I28" s="0" t="n">
-        <v>196</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="0" t="s">
         <v>37</v>
       </c>
@@ -1380,7 +1243,7 @@
         <v>643</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>511.33000000000004</v>
+        <v>511.33</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>12269</v>
@@ -1394,14 +1257,8 @@
       <c r="H29" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="I29" s="0" t="n">
-        <v>555</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="0" t="s">
         <v>38</v>
       </c>
@@ -1412,7 +1269,7 @@
         <v>311</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>156.67999999999984</v>
+        <v>156.67999999999986</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>3755</v>
@@ -1426,14 +1283,8 @@
       <c r="H30" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="I30" s="0" t="n">
-        <v>182</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="0" t="s">
         <v>39</v>
       </c>
@@ -1444,7 +1295,7 @@
         <v>111</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>98.22000000000003</v>
+        <v>98.22000000000001</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>2357</v>
@@ -1458,14 +1309,8 @@
       <c r="H31" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I31" s="0" t="n">
-        <v>110</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="0" t="s">
         <v>40</v>
       </c>
@@ -1476,7 +1321,7 @@
         <v>202</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>150.28999999999996</v>
+        <v>150.29</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>3606</v>
@@ -1490,14 +1335,8 @@
       <c r="H32" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I32" s="0" t="n">
-        <v>163</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="0" t="s">
         <v>41</v>
       </c>
@@ -1522,14 +1361,8 @@
       <c r="H33" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I33" s="0" t="n">
-        <v>98</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="0" t="s">
         <v>42</v>
       </c>
@@ -1540,7 +1373,7 @@
         <v>339</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>216.70999999999995</v>
+        <v>216.70999999999998</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>5198</v>
@@ -1554,14 +1387,8 @@
       <c r="H34" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I34" s="0" t="n">
-        <v>254</v>
-      </c>
-      <c r="J34" s="0" t="n">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="0" t="s">
         <v>43</v>
       </c>
@@ -1572,7 +1399,7 @@
         <v>331</v>
       </c>
       <c r="D35" s="0" t="n">
-        <v>267.59999999999997</v>
+        <v>267.6</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>6421</v>
@@ -1586,14 +1413,8 @@
       <c r="H35" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I35" s="0" t="n">
-        <v>294</v>
-      </c>
-      <c r="J35" s="0" t="n">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="0" t="s">
         <v>44</v>
       </c>
@@ -1618,14 +1439,8 @@
       <c r="H36" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I36" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="J36" s="0" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="0" t="s">
         <v>45</v>
       </c>
@@ -1636,7 +1451,7 @@
         <v>239</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>222.54000000000002</v>
+        <v>222.54</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>5340</v>
@@ -1650,14 +1465,8 @@
       <c r="H37" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I37" s="0" t="n">
-        <v>236</v>
-      </c>
-      <c r="J37" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="0" t="s">
         <v>46</v>
       </c>
@@ -1668,7 +1477,7 @@
         <v>271</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>174.86999999999998</v>
+        <v>174.8699999999999</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>4194</v>
@@ -1682,14 +1491,8 @@
       <c r="H38" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I38" s="0" t="n">
-        <v>185</v>
-      </c>
-      <c r="J38" s="0" t="n">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="0" t="s">
         <v>47</v>
       </c>
@@ -1700,7 +1503,7 @@
         <v>480</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>277.92999999999955</v>
+        <v>277.9300000000002</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>6665</v>
@@ -1714,14 +1517,8 @@
       <c r="H39" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="I39" s="0" t="n">
-        <v>301</v>
-      </c>
-      <c r="J39" s="0" t="n">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="0" t="s">
         <v>48</v>
       </c>
@@ -1732,7 +1529,7 @@
         <v>108</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>55.890000000000015</v>
+        <v>55.89000000000001</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>1340</v>
@@ -1746,14 +1543,8 @@
       <c r="H40" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I40" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="J40" s="0" t="n">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="0" t="s">
         <v>49</v>
       </c>
@@ -1778,14 +1569,8 @@
       <c r="H41" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I41" s="0" t="n">
-        <v>180</v>
-      </c>
-      <c r="J41" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="0" t="s">
         <v>50</v>
       </c>
@@ -1796,7 +1581,7 @@
         <v>304</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>170.82999999999993</v>
+        <v>170.82999999999996</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>4098</v>
@@ -1810,14 +1595,8 @@
       <c r="H42" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="I42" s="0" t="n">
-        <v>181</v>
-      </c>
-      <c r="J42" s="0" t="n">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="0" t="s">
         <v>51</v>
       </c>
@@ -1828,7 +1607,7 @@
         <v>260</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>73.71</v>
+        <v>73.71000000000004</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>1766</v>
@@ -1842,14 +1621,8 @@
       <c r="H43" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="I43" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="J43" s="0" t="n">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="0" t="s">
         <v>52</v>
       </c>
@@ -1860,7 +1633,7 @@
         <v>465</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>345.54999999999984</v>
+        <v>345.5499999999998</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>8290</v>
@@ -1874,14 +1647,8 @@
       <c r="H44" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="I44" s="0" t="n">
-        <v>381</v>
-      </c>
-      <c r="J44" s="0" t="n">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="0" t="s">
         <v>53</v>
       </c>
@@ -1906,14 +1673,8 @@
       <c r="H45" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I45" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="J45" s="0" t="n">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="0" t="s">
         <v>54</v>
       </c>
@@ -1924,7 +1685,7 @@
         <v>155</v>
       </c>
       <c r="D46" s="0" t="n">
-        <v>70.69999999999999</v>
+        <v>70.7</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>1694</v>
@@ -1938,14 +1699,8 @@
       <c r="H46" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I46" s="0" t="n">
-        <v>68</v>
-      </c>
-      <c r="J46" s="0" t="n">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="0" t="s">
         <v>55</v>
       </c>
@@ -1956,7 +1711,7 @@
         <v>430</v>
       </c>
       <c r="D47" s="0" t="n">
-        <v>251.56999999999977</v>
+        <v>251.56999999999974</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>6033</v>
@@ -1970,14 +1725,8 @@
       <c r="H47" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I47" s="0" t="n">
-        <v>292</v>
-      </c>
-      <c r="J47" s="0" t="n">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="0" t="s">
         <v>56</v>
       </c>
@@ -2002,14 +1751,8 @@
       <c r="H48" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I48" s="0" t="n">
-        <v>112</v>
-      </c>
-      <c r="J48" s="0" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="0" t="s">
         <v>57</v>
       </c>
@@ -2034,14 +1777,8 @@
       <c r="H49" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I49" s="0" t="n">
-        <v>200</v>
-      </c>
-      <c r="J49" s="0" t="n">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="0" t="s">
         <v>58</v>
       </c>
@@ -2052,7 +1789,7 @@
         <v>186</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>103.02</v>
+        <v>103.01999999999997</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>2471</v>
@@ -2066,14 +1803,8 @@
       <c r="H50" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I50" s="0" t="n">
-        <v>115</v>
-      </c>
-      <c r="J50" s="0" t="n">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="0" t="s">
         <v>59</v>
       </c>
@@ -2098,14 +1829,8 @@
       <c r="H51" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I51" s="0" t="n">
-        <v>194</v>
-      </c>
-      <c r="J51" s="0" t="n">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="0" t="s">
         <v>60</v>
       </c>
@@ -2130,14 +1855,8 @@
       <c r="H52" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I52" s="0" t="n">
-        <v>103</v>
-      </c>
-      <c r="J52" s="0" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="0" t="s">
         <v>61</v>
       </c>
@@ -2148,7 +1867,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>35.919999999999995</v>
+        <v>35.92</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>861</v>
@@ -2162,14 +1881,8 @@
       <c r="H53" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I53" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="J53" s="0" t="n">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="0" t="s">
         <v>62</v>
       </c>
@@ -2180,7 +1893,7 @@
         <v>267</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>198.02999999999997</v>
+        <v>198.02999999999992</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>4750</v>
@@ -2194,14 +1907,8 @@
       <c r="H54" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="I54" s="0" t="n">
-        <v>241</v>
-      </c>
-      <c r="J54" s="0" t="n">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="0" t="s">
         <v>63</v>
       </c>
@@ -2212,7 +1919,7 @@
         <v>209</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>128.69000000000008</v>
+        <v>128.69000000000005</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>3087</v>
@@ -2226,14 +1933,8 @@
       <c r="H55" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I55" s="0" t="n">
-        <v>144</v>
-      </c>
-      <c r="J55" s="0" t="n">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="0" t="s">
         <v>64</v>
       </c>
@@ -2258,14 +1959,8 @@
       <c r="H56" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="I56" s="0" t="n">
-        <v>133</v>
-      </c>
-      <c r="J56" s="0" t="n">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="0" t="s">
         <v>65</v>
       </c>
@@ -2290,14 +1985,8 @@
       <c r="H57" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I57" s="0" t="n">
-        <v>74</v>
-      </c>
-      <c r="J57" s="0" t="n">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="0" t="s">
         <v>66</v>
       </c>
@@ -2308,7 +1997,7 @@
         <v>48</v>
       </c>
       <c r="D58" s="0" t="n">
-        <v>30.45</v>
+        <v>30.450000000000003</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>730</v>
@@ -2322,14 +2011,8 @@
       <c r="H58" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I58" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="J58" s="0" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="0" t="s">
         <v>67</v>
       </c>
@@ -2354,14 +2037,8 @@
       <c r="H59" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I59" s="0" t="n">
-        <v>234</v>
-      </c>
-      <c r="J59" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="0" t="s">
         <v>68</v>
       </c>
@@ -2386,14 +2063,8 @@
       <c r="H60" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I60" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="J60" s="0" t="n">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="0" t="s">
         <v>69</v>
       </c>
@@ -2404,7 +2075,7 @@
         <v>192</v>
       </c>
       <c r="D61" s="0" t="n">
-        <v>147.85999999999999</v>
+        <v>147.86000000000004</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>3548</v>
@@ -2418,14 +2089,8 @@
       <c r="H61" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I61" s="0" t="n">
-        <v>158</v>
-      </c>
-      <c r="J61" s="0" t="n">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="0" t="s">
         <v>70</v>
       </c>
@@ -2450,14 +2115,8 @@
       <c r="H62" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="I62" s="0" t="n">
-        <v>391</v>
-      </c>
-      <c r="J62" s="0" t="n">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="0" t="s">
         <v>71</v>
       </c>
@@ -2468,7 +2127,7 @@
         <v>268</v>
       </c>
       <c r="D63" s="0" t="n">
-        <v>161.07999999999998</v>
+        <v>161.07999999999996</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>3864</v>
@@ -2482,14 +2141,8 @@
       <c r="H63" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I63" s="0" t="n">
-        <v>172</v>
-      </c>
-      <c r="J63" s="0" t="n">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="0" t="s">
         <v>72</v>
       </c>
@@ -2514,14 +2167,8 @@
       <c r="H64" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I64" s="0" t="n">
-        <v>271</v>
-      </c>
-      <c r="J64" s="0" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="0" t="s">
         <v>73</v>
       </c>
@@ -2546,14 +2193,8 @@
       <c r="H65" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I65" s="0" t="n">
-        <v>23</v>
-      </c>
-      <c r="J65" s="0" t="n">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="0" t="s">
         <v>74</v>
       </c>
@@ -2578,14 +2219,8 @@
       <c r="H66" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I66" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="J66" s="0" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="0" t="s">
         <v>75</v>
       </c>
@@ -2596,7 +2231,7 @@
         <v>287</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>209.4</v>
+        <v>209.40000000000003</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>5025</v>
@@ -2610,14 +2245,8 @@
       <c r="H67" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I67" s="0" t="n">
-        <v>240</v>
-      </c>
-      <c r="J67" s="0" t="n">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="0" t="s">
         <v>76</v>
       </c>
@@ -2628,7 +2257,7 @@
         <v>184</v>
       </c>
       <c r="D68" s="0" t="n">
-        <v>124.62999999999998</v>
+        <v>124.62999999999995</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>2989</v>
@@ -2642,14 +2271,8 @@
       <c r="H68" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I68" s="0" t="n">
-        <v>137</v>
-      </c>
-      <c r="J68" s="0" t="n">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="0" t="s">
         <v>77</v>
       </c>
@@ -2660,7 +2283,7 @@
         <v>66</v>
       </c>
       <c r="D69" s="0" t="n">
-        <v>23.729999999999997</v>
+        <v>23.729999999999993</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>569</v>
@@ -2674,14 +2297,8 @@
       <c r="H69" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I69" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="J69" s="0" t="n">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="0" t="s">
         <v>78</v>
       </c>
@@ -2692,7 +2309,7 @@
         <v>503</v>
       </c>
       <c r="D70" s="0" t="n">
-        <v>272.0599999999999</v>
+        <v>272.0599999999998</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>6525</v>
@@ -2706,14 +2323,8 @@
       <c r="H70" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I70" s="0" t="n">
-        <v>280</v>
-      </c>
-      <c r="J70" s="0" t="n">
-        <v>1129</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="0" t="s">
         <v>79</v>
       </c>
@@ -2724,7 +2335,7 @@
         <v>93</v>
       </c>
       <c r="D71" s="0" t="n">
-        <v>52.98</v>
+        <v>52.980000000000004</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>1271</v>
@@ -2738,14 +2349,8 @@
       <c r="H71" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I71" s="0" t="n">
-        <v>58</v>
-      </c>
-      <c r="J71" s="0" t="n">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="0" t="s">
         <v>80</v>
       </c>
@@ -2770,14 +2375,8 @@
       <c r="H72" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I72" s="0" t="n">
-        <v>160</v>
-      </c>
-      <c r="J72" s="0" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="0" t="s">
         <v>81</v>
       </c>
@@ -2788,7 +2387,7 @@
         <v>188</v>
       </c>
       <c r="D73" s="0" t="n">
-        <v>146.27000000000004</v>
+        <v>146.27</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>3510</v>
@@ -2802,14 +2401,8 @@
       <c r="H73" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I73" s="0" t="n">
-        <v>167</v>
-      </c>
-      <c r="J73" s="0" t="n">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="0" t="s">
         <v>82</v>
       </c>
@@ -2820,7 +2413,7 @@
         <v>104</v>
       </c>
       <c r="D74" s="0" t="n">
-        <v>76.00999999999998</v>
+        <v>76.00999999999999</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>1824</v>
@@ -2834,14 +2427,8 @@
       <c r="H74" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I74" s="0" t="n">
-        <v>83</v>
-      </c>
-      <c r="J74" s="0" t="n">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="0" t="s">
         <v>83</v>
       </c>
@@ -2866,14 +2453,8 @@
       <c r="H75" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I75" s="0" t="n">
-        <v>191</v>
-      </c>
-      <c r="J75" s="0" t="n">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="0" t="s">
         <v>84</v>
       </c>
@@ -2884,7 +2465,7 @@
         <v>259</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>122.48999999999995</v>
+        <v>122.48999999999997</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>2937</v>
@@ -2898,14 +2479,8 @@
       <c r="H76" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="I76" s="0" t="n">
-        <v>134</v>
-      </c>
-      <c r="J76" s="0" t="n">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="0" t="s">
         <v>85</v>
       </c>
@@ -2916,7 +2491,7 @@
         <v>246</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>123.24000000000014</v>
+        <v>123.24000000000015</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>2955</v>
@@ -2930,14 +2505,8 @@
       <c r="H77" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I77" s="0" t="n">
-        <v>135</v>
-      </c>
-      <c r="J77" s="0" t="n">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="0" t="s">
         <v>86</v>
       </c>
@@ -2948,7 +2517,7 @@
         <v>287</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>166.63999999999996</v>
+        <v>166.63999999999993</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>3998</v>
@@ -2962,14 +2531,8 @@
       <c r="H78" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I78" s="0" t="n">
-        <v>184</v>
-      </c>
-      <c r="J78" s="0" t="n">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="0" t="s">
         <v>87</v>
       </c>
@@ -2980,7 +2543,7 @@
         <v>282</v>
       </c>
       <c r="D79" s="0" t="n">
-        <v>155.79999999999993</v>
+        <v>155.7999999999998</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>3738</v>
@@ -2994,14 +2557,8 @@
       <c r="H79" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I79" s="0" t="n">
-        <v>155</v>
-      </c>
-      <c r="J79" s="0" t="n">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="0" t="s">
         <v>88</v>
       </c>
@@ -3026,14 +2583,8 @@
       <c r="H80" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I80" s="0" t="n">
-        <v>144</v>
-      </c>
-      <c r="J80" s="0" t="n">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="0" t="s">
         <v>89</v>
       </c>
@@ -3044,7 +2595,7 @@
         <v>45</v>
       </c>
       <c r="D81" s="0" t="n">
-        <v>34.53</v>
+        <v>34.529999999999994</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>829</v>
@@ -3058,14 +2609,8 @@
       <c r="H81" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I81" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="J81" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="0" t="s">
         <v>90</v>
       </c>
@@ -3076,7 +2621,7 @@
         <v>524</v>
       </c>
       <c r="D82" s="0" t="n">
-        <v>269.23999999999967</v>
+        <v>269.2399999999997</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>6459</v>
@@ -3090,14 +2635,8 @@
       <c r="H82" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="I82" s="0" t="n">
-        <v>277</v>
-      </c>
-      <c r="J82" s="0" t="n">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="0" t="s">
         <v>91</v>
       </c>
@@ -3122,14 +2661,8 @@
       <c r="H83" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="I83" s="0" t="n">
-        <v>136</v>
-      </c>
-      <c r="J83" s="0" t="n">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="0" t="s">
         <v>92</v>
       </c>
@@ -3154,14 +2687,8 @@
       <c r="H84" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I84" s="0" t="n">
-        <v>156</v>
-      </c>
-      <c r="J84" s="0" t="n">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="0" t="s">
         <v>93</v>
       </c>
@@ -3186,14 +2713,8 @@
       <c r="H85" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="I85" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="J85" s="0" t="n">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="0" t="s">
         <v>94</v>
       </c>
@@ -3204,7 +2725,7 @@
         <v>353</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>202.78999999999985</v>
+        <v>202.7899999999997</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>4863</v>
@@ -3218,14 +2739,8 @@
       <c r="H86" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="I86" s="0" t="n">
-        <v>229</v>
-      </c>
-      <c r="J86" s="0" t="n">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="0" t="s">
         <v>95</v>
       </c>
@@ -3250,14 +2765,8 @@
       <c r="H87" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I87" s="0" t="n">
-        <v>139</v>
-      </c>
-      <c r="J87" s="0" t="n">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" s="0" t="s">
         <v>96</v>
       </c>
@@ -3268,7 +2777,7 @@
         <v>220</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>142.79000000000002</v>
+        <v>142.79</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>3425</v>
@@ -3282,14 +2791,8 @@
       <c r="H88" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I88" s="0" t="n">
-        <v>164</v>
-      </c>
-      <c r="J88" s="0" t="n">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" s="0" t="s">
         <v>97</v>
       </c>
@@ -3314,14 +2817,8 @@
       <c r="H89" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="I89" s="0" t="n">
-        <v>66</v>
-      </c>
-      <c r="J89" s="0" t="n">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="0" t="s">
         <v>98</v>
       </c>
@@ -3332,7 +2829,7 @@
         <v>169</v>
       </c>
       <c r="D90" s="0" t="n">
-        <v>63.70000000000001</v>
+        <v>63.7</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>1527</v>
@@ -3346,14 +2843,8 @@
       <c r="H90" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I90" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="J90" s="0" t="n">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="0" t="s">
         <v>99</v>
       </c>
@@ -3378,14 +2869,8 @@
       <c r="H91" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I91" s="0" t="n">
-        <v>299</v>
-      </c>
-      <c r="J91" s="0" t="n">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" s="0" t="s">
         <v>100</v>
       </c>
@@ -3396,7 +2881,7 @@
         <v>211</v>
       </c>
       <c r="D92" s="0" t="n">
-        <v>143.28999999999994</v>
+        <v>143.29</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>3438</v>
@@ -3410,14 +2895,8 @@
       <c r="H92" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I92" s="0" t="n">
-        <v>163</v>
-      </c>
-      <c r="J92" s="0" t="n">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10">
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" s="0" t="s">
         <v>101</v>
       </c>
@@ -3442,14 +2921,8 @@
       <c r="H93" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I93" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="J93" s="0" t="n">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10">
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" s="0" t="s">
         <v>102</v>
       </c>
@@ -3474,14 +2947,8 @@
       <c r="H94" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I94" s="0" t="n">
-        <v>123</v>
-      </c>
-      <c r="J94" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10">
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="0" t="s">
         <v>103</v>
       </c>
@@ -3506,14 +2973,8 @@
       <c r="H95" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I95" s="0" t="n">
-        <v>169</v>
-      </c>
-      <c r="J95" s="0" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" s="0" t="s">
         <v>104</v>
       </c>
@@ -3524,7 +2985,7 @@
         <v>177</v>
       </c>
       <c r="D96" s="0" t="n">
-        <v>84.28999999999996</v>
+        <v>84.29</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>2021</v>
@@ -3538,14 +2999,8 @@
       <c r="H96" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I96" s="0" t="n">
-        <v>87</v>
-      </c>
-      <c r="J96" s="0" t="n">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10">
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="0" t="s">
         <v>105</v>
       </c>
@@ -3556,7 +3011,7 @@
         <v>67</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>31.150000000000002</v>
+        <v>31.149999999999995</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>746</v>
@@ -3570,14 +3025,8 @@
       <c r="H97" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I97" s="0" t="n">
-        <v>30</v>
-      </c>
-      <c r="J97" s="0" t="n">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10">
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="0" t="s">
         <v>106</v>
       </c>
@@ -3588,7 +3037,7 @@
         <v>121</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>67.92000000000003</v>
+        <v>67.92000000000002</v>
       </c>
       <c r="E98" s="0" t="n">
         <v>1628</v>
@@ -3602,14 +3051,8 @@
       <c r="H98" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="I98" s="0" t="n">
-        <v>78</v>
-      </c>
-      <c r="J98" s="0" t="n">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10">
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="0" t="s">
         <v>107</v>
       </c>
@@ -3620,7 +3063,7 @@
         <v>210</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>123.21999999999991</v>
+        <v>123.21999999999993</v>
       </c>
       <c r="E99" s="0" t="n">
         <v>2957</v>
@@ -3634,14 +3077,8 @@
       <c r="H99" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I99" s="0" t="n">
-        <v>139</v>
-      </c>
-      <c r="J99" s="0" t="n">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10">
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" s="0" t="s">
         <v>108</v>
       </c>
@@ -3666,14 +3103,8 @@
       <c r="H100" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I100" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="J100" s="0" t="n">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10">
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" s="0" t="s">
         <v>109</v>
       </c>
@@ -3698,14 +3129,8 @@
       <c r="H101" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I101" s="0" t="n">
-        <v>82</v>
-      </c>
-      <c r="J101" s="0" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10">
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" s="0" t="s">
         <v>110</v>
       </c>
@@ -3716,7 +3141,7 @@
         <v>27</v>
       </c>
       <c r="D102" s="0" t="n">
-        <v>13.45</v>
+        <v>13.450000000000001</v>
       </c>
       <c r="E102" s="0" t="n">
         <v>322</v>
@@ -3730,14 +3155,8 @@
       <c r="H102" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I102" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J102" s="0" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10">
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" s="0" t="s">
         <v>111</v>
       </c>
@@ -3748,7 +3167,7 @@
         <v>179</v>
       </c>
       <c r="D103" s="0" t="n">
-        <v>42.090000000000025</v>
+        <v>42.09</v>
       </c>
       <c r="E103" s="0" t="n">
         <v>1006</v>
@@ -3762,14 +3181,8 @@
       <c r="H103" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I103" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="J103" s="0" t="n">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10">
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" s="0" t="s">
         <v>112</v>
       </c>
@@ -3794,14 +3207,8 @@
       <c r="H104" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I104" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="J104" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10">
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" s="0" t="s">
         <v>113</v>
       </c>
@@ -3812,7 +3219,7 @@
         <v>86</v>
       </c>
       <c r="D105" s="0" t="n">
-        <v>42.31999999999999</v>
+        <v>42.320000000000014</v>
       </c>
       <c r="E105" s="0" t="n">
         <v>1014</v>
@@ -3826,14 +3233,8 @@
       <c r="H105" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I105" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="J105" s="0" t="n">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10">
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" s="0" t="s">
         <v>114</v>
       </c>
@@ -3858,14 +3259,8 @@
       <c r="H106" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I106" s="0" t="n">
-        <v>123</v>
-      </c>
-      <c r="J106" s="0" t="n">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10">
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" s="0" t="s">
         <v>115</v>
       </c>
@@ -3876,7 +3271,7 @@
         <v>290</v>
       </c>
       <c r="D107" s="0" t="n">
-        <v>193.92999999999992</v>
+        <v>193.92999999999995</v>
       </c>
       <c r="E107" s="0" t="n">
         <v>4654</v>
@@ -3890,14 +3285,8 @@
       <c r="H107" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="I107" s="0" t="n">
-        <v>205</v>
-      </c>
-      <c r="J107" s="0" t="n">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10">
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" s="0" t="s">
         <v>116</v>
       </c>
@@ -3908,7 +3297,7 @@
         <v>81</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>33.55</v>
+        <v>33.54999999999999</v>
       </c>
       <c r="E108" s="0" t="n">
         <v>804</v>
@@ -3922,14 +3311,8 @@
       <c r="H108" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I108" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="J108" s="0" t="n">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" s="0" t="s">
         <v>117</v>
       </c>
@@ -3954,14 +3337,8 @@
       <c r="H109" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="I109" s="0" t="n">
-        <v>195</v>
-      </c>
-      <c r="J109" s="0" t="n">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10">
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" s="0" t="s">
         <v>118</v>
       </c>
@@ -3972,7 +3349,7 @@
         <v>463</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>301.3499999999998</v>
+        <v>301.3499999999999</v>
       </c>
       <c r="E110" s="0" t="n">
         <v>7227</v>
@@ -3986,14 +3363,8 @@
       <c r="H110" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="I110" s="0" t="n">
-        <v>348</v>
-      </c>
-      <c r="J110" s="0" t="n">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10">
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" s="0" t="s">
         <v>119</v>
       </c>
@@ -4004,7 +3375,7 @@
         <v>239</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>195.99999999999994</v>
+        <v>195.9999999999999</v>
       </c>
       <c r="E111" s="0" t="n">
         <v>4703</v>
@@ -4018,14 +3389,8 @@
       <c r="H111" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I111" s="0" t="n">
-        <v>208</v>
-      </c>
-      <c r="J111" s="0" t="n">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10">
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" s="0" t="s">
         <v>120</v>
       </c>
@@ -4050,14 +3415,8 @@
       <c r="H112" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="I112" s="0" t="n">
-        <v>69</v>
-      </c>
-      <c r="J112" s="0" t="n">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10">
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" s="0" t="s">
         <v>121</v>
       </c>
@@ -4068,7 +3427,7 @@
         <v>57</v>
       </c>
       <c r="D113" s="0" t="n">
-        <v>39.089999999999996</v>
+        <v>39.08999999999999</v>
       </c>
       <c r="E113" s="0" t="n">
         <v>938</v>
@@ -4082,14 +3441,8 @@
       <c r="H113" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I113" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="J113" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10">
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114" s="0" t="s">
         <v>122</v>
       </c>
@@ -4100,7 +3453,7 @@
         <v>240</v>
       </c>
       <c r="D114" s="0" t="n">
-        <v>165.25000000000003</v>
+        <v>165.25000000000006</v>
       </c>
       <c r="E114" s="0" t="n">
         <v>3965</v>
@@ -4114,14 +3467,8 @@
       <c r="H114" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I114" s="0" t="n">
-        <v>170</v>
-      </c>
-      <c r="J114" s="0" t="n">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10">
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115" s="0" t="s">
         <v>123</v>
       </c>
@@ -4132,7 +3479,7 @@
         <v>242</v>
       </c>
       <c r="D115" s="0" t="n">
-        <v>133.95000000000002</v>
+        <v>133.95000000000007</v>
       </c>
       <c r="E115" s="0" t="n">
         <v>3214</v>
@@ -4146,14 +3493,8 @@
       <c r="H115" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="I115" s="0" t="n">
-        <v>155</v>
-      </c>
-      <c r="J115" s="0" t="n">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10">
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116" s="0" t="s">
         <v>124</v>
       </c>
@@ -4164,7 +3505,7 @@
         <v>212</v>
       </c>
       <c r="D116" s="0" t="n">
-        <v>87.61000000000001</v>
+        <v>87.61000000000004</v>
       </c>
       <c r="E116" s="0" t="n">
         <v>2100</v>
@@ -4178,14 +3519,8 @@
       <c r="H116" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="I116" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="J116" s="0" t="n">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10">
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117" s="0" t="s">
         <v>125</v>
       </c>
@@ -4196,7 +3531,7 @@
         <v>270</v>
       </c>
       <c r="D117" s="0" t="n">
-        <v>166.00000000000009</v>
+        <v>166.00000000000003</v>
       </c>
       <c r="E117" s="0" t="n">
         <v>3982</v>
@@ -4210,14 +3545,8 @@
       <c r="H117" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="I117" s="0" t="n">
-        <v>185</v>
-      </c>
-      <c r="J117" s="0" t="n">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10">
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" s="0" t="s">
         <v>126</v>
       </c>
@@ -4228,7 +3557,7 @@
         <v>130</v>
       </c>
       <c r="D118" s="0" t="n">
-        <v>116.30000000000003</v>
+        <v>116.3</v>
       </c>
       <c r="E118" s="0" t="n">
         <v>2791</v>
@@ -4242,14 +3571,8 @@
       <c r="H118" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I118" s="0" t="n">
-        <v>125</v>
-      </c>
-      <c r="J118" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10">
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" s="0" t="s">
         <v>127</v>
       </c>
@@ -4260,7 +3583,7 @@
         <v>53</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>43.31</v>
+        <v>43.309999999999995</v>
       </c>
       <c r="E119" s="0" t="n">
         <v>1039</v>
@@ -4274,14 +3597,8 @@
       <c r="H119" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I119" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="J119" s="0" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10">
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" s="0" t="s">
         <v>128</v>
       </c>
@@ -4292,7 +3609,7 @@
         <v>59</v>
       </c>
       <c r="D120" s="0" t="n">
-        <v>37.39000000000001</v>
+        <v>37.39</v>
       </c>
       <c r="E120" s="0" t="n">
         <v>896</v>
@@ -4306,14 +3623,8 @@
       <c r="H120" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I120" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="J120" s="0" t="n">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10">
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" s="0" t="s">
         <v>129</v>
       </c>
@@ -4338,14 +3649,8 @@
       <c r="H121" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="I121" s="0" t="n">
-        <v>169</v>
-      </c>
-      <c r="J121" s="0" t="n">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10">
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" s="0" t="s">
         <v>130</v>
       </c>
@@ -4370,14 +3675,8 @@
       <c r="H122" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I122" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J122" s="0" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10">
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" s="0" t="s">
         <v>131</v>
       </c>
@@ -4402,14 +3701,8 @@
       <c r="H123" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I123" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J123" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10">
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124" s="0" t="s">
         <v>132</v>
       </c>
@@ -4434,14 +3727,8 @@
       <c r="H124" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I124" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="J124" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10">
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" s="0" t="s">
         <v>133</v>
       </c>
@@ -4466,14 +3753,8 @@
       <c r="H125" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="I125" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="J125" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10">
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" s="0" t="s">
         <v>134</v>
       </c>
@@ -4498,14 +3779,8 @@
       <c r="H126" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I126" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="J126" s="0" t="n">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10">
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127" s="0" t="s">
         <v>135</v>
       </c>
@@ -4516,7 +3791,7 @@
         <v>112</v>
       </c>
       <c r="D127" s="0" t="n">
-        <v>40.830000000000005</v>
+        <v>40.83</v>
       </c>
       <c r="E127" s="0" t="n">
         <v>978</v>
@@ -4530,14 +3805,8 @@
       <c r="H127" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="I127" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="J127" s="0" t="n">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10">
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" s="0" t="s">
         <v>136</v>
       </c>
@@ -4562,14 +3831,8 @@
       <c r="H128" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I128" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="J128" s="0" t="n">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10">
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129" s="0" t="s">
         <v>137</v>
       </c>
@@ -4580,7 +3843,7 @@
         <v>32</v>
       </c>
       <c r="D129" s="0" t="n">
-        <v>6.17</v>
+        <v>6.170000000000001</v>
       </c>
       <c r="E129" s="0" t="n">
         <v>148</v>
@@ -4594,14 +3857,8 @@
       <c r="H129" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I129" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J129" s="0" t="n">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10">
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" s="0" t="s">
         <v>138</v>
       </c>
@@ -4612,7 +3869,7 @@
         <v>37</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>25.869999999999994</v>
+        <v>25.869999999999997</v>
       </c>
       <c r="E130" s="0" t="n">
         <v>621</v>
@@ -4626,11 +3883,148 @@
       <c r="H130" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I130" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="J130" s="0" t="n">
-        <v>25</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1362</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1335269</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>215304</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>9665</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>8972.03</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>921</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2657</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>721043</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>105543</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5944</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>4399.5</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>2119</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3116</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>376102</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>52903</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>3116</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>2206.11</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>2719</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>8445</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>283116</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>39133</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>8444</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>1634.35</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>6871</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>